<commit_message>
Sankey All Elc Sector fix
</commit_message>
<xml_diff>
--- a/LMADefs-SATIMGE.xlsx
+++ b/LMADefs-SATIMGE.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AC6395-98E1-4AC4-B0B5-8678CC93B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E36E12-1009-46B0-92CB-DE10352305BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3045" yWindow="-20175" windowWidth="28350" windowHeight="15150" firstSheet="1" activeTab="3" xr2:uid="{05AD35DE-0BB5-4D70-AD01-E84E11ACA14E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{05AD35DE-0BB5-4D70-AD01-E84E11ACA14E}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
     <sheet name="TS_Defs" sheetId="27" r:id="rId2"/>
     <sheet name="TS_Defs_Old" sheetId="70" r:id="rId3"/>
-    <sheet name="TS_Defs_Sankey" sheetId="71" r:id="rId4"/>
+    <sheet name="Sankey_def" sheetId="71" r:id="rId4"/>
     <sheet name="PSet_MAP coarse" sheetId="57" r:id="rId5"/>
     <sheet name="CSET_MAP" sheetId="66" r:id="rId6"/>
     <sheet name="TS ratios" sheetId="68" r:id="rId7"/>
@@ -29,9 +29,9 @@
     <sheet name="UnitConv" sheetId="59" r:id="rId14"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sankey_def!$A$2:$N$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TS_Defs!$A$2:$O$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TS_Defs_Old!$A$2:$N$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TS_Defs_Sankey!$A$2:$N$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3738,13 +3738,13 @@
     <t>Cooking,Lighting,Other,Refrigeration,Space Heating,Water Heating,</t>
   </si>
   <si>
-    <t>TS_Defs: snk_attr=Sankey_ResDetV0</t>
-  </si>
-  <si>
     <t>~TS_Defs: snk_attr=Sankey_ResDetV1</t>
   </si>
   <si>
     <t>TS_Defs: snk_attr=Sankey_ResDetV2</t>
+  </si>
+  <si>
+    <t>~TS_Defs: snk_attr=Sankey_Test</t>
   </si>
 </sst>
 </file>
@@ -29366,15 +29366,15 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -29463,7 +29463,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>1018</v>
       </c>
       <c r="H3" t="s">
         <v>1067</v>
@@ -29641,7 +29641,7 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -29790,7 +29790,7 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -29964,7 +29964,7 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="43" spans="1:19">

</xml_diff>

<commit_message>
Industry test for sankey
</commit_message>
<xml_diff>
--- a/LMADefs-SATIMGE.xlsx
+++ b/LMADefs-SATIMGE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\Workooks for VEDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26849F52-0F69-4CE6-8D38-AED857F10C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF935E-C0F1-4F48-AF3C-2F7FC7469A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="-18525" windowWidth="28695" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{05AD35DE-0BB5-4D70-AD01-E84E11ACA14E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{05AD35DE-0BB5-4D70-AD01-E84E11ACA14E}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -34,18 +34,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TS_Defs!$A$2:$O$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TS_Defs_Old!$A$2:$N$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -432,12 +421,63 @@
         </r>
       </text>
     </comment>
+    <comment ref="B65" authorId="0" shapeId="0" xr:uid="{7158817D-962F-41B1-9F6C-927F7BAF6810}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amit Kanudia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3/20/2013
+to use as weight for aggregating over commodities or TS (or process?)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{BCA3E373-85D0-48BF-A6E9-829E0752AF7E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amit Kanudia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+6/4/2011
+These sets should not have common elements</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="363">
   <si>
     <t>Unit</t>
   </si>
@@ -1505,6 +1545,27 @@
   </si>
   <si>
     <t>Electrolysers,FuelCells,Aluminium,Chemicals,Ammonia,FerroAlloys,Food_Bev_Tob,Iron_Steel,Mining,PNFMetals,NMMProducts,IndOther,PGM,Pulp_Paper,</t>
+  </si>
+  <si>
+    <t>~TS_Defs: snk_attr=Sankey_Industry_Other</t>
+  </si>
+  <si>
+    <t>Industry,HydrogenSector,FuelSupply,Electrolysers,FuelCells,Aluminium,Chemicals,Ammonia,FerroAlloys,Food_Bev_Tob,Iron_Steel,Mining,PNFMetals,NMMProducts,IndOther,PGM,Pulp_Paper,ProcessHeat,PumpsFansCompressors,Lighting,Space Heating,Other,IndTransport,Cooling</t>
+  </si>
+  <si>
+    <t>ProcessHeat,PumpsFansCompressors,Lighting,Space Heating,Other,IndTransport,Cooling</t>
+  </si>
+  <si>
+    <t>Lighting dem,Other dem,Space Heating dem,Electricity Heating dem,PumpsFansCompressors dem,Cooling dem,Process Heating dem,Transport Services</t>
+  </si>
+  <si>
+    <t>Industry,HydrogenSector,FuelSupply,Electrolysers,FuelCells,Aluminium,Chemicals,Ammonia,FerroAlloys,Food_Bev_Tob,Iron_Steel,Mining,PNFMetals,NMMProducts,IndOther,PGM,Pulp_Paper</t>
+  </si>
+  <si>
+    <t>Hydrogen,NaturalGas,Coal,OilProducts,Biomass,Lighting dem,Other dem,Space Heating dem,Electricity Heating dem,PumpsFansCompressors dem,Cooling dem,Process Heating dem,Transport Services</t>
+  </si>
+  <si>
+    <t>ElectricityDist,Hydrogen,NaturalGas,Coal,OilProducts,Biomass</t>
   </si>
 </sst>
 </file>
@@ -1516,7 +1577,7 @@
     <numFmt numFmtId="165" formatCode="#.00"/>
     <numFmt numFmtId="166" formatCode="#."/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1619,6 +1680,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1671,11 +1752,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Date" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2000,7 +2085,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3579,7 +3664,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="C57" sqref="C57:D68"/>
     </sheetView>
   </sheetViews>
@@ -5032,10 +5117,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17EB7CB0-10A4-4243-B0C4-E7A691753461}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59:S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5928,16 +6013,364 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
-      <c r="K59" t="s">
+    <row r="64" spans="1:19">
+      <c r="A64" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
+      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" s="5" customFormat="1">
+      <c r="A66" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" t="s">
+        <v>270</v>
+      </c>
+      <c r="I66" s="7"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N59" t="s">
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+    </row>
+    <row r="67" spans="1:20" s="5" customFormat="1">
+      <c r="A67" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" t="s">
+        <v>270</v>
+      </c>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
+    </row>
+    <row r="68" spans="1:20" s="5" customFormat="1">
+      <c r="A68" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+    </row>
+    <row r="69" spans="1:20" s="5" customFormat="1">
+      <c r="A69" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" t="s">
+        <v>362</v>
+      </c>
+      <c r="I69" s="7"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+    </row>
+    <row r="70" spans="1:20">
+      <c r="A70" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" t="s">
+        <v>361</v>
+      </c>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S70" s="6"/>
+      <c r="T70" s="6"/>
+    </row>
+    <row r="71" spans="1:20" s="5" customFormat="1">
+      <c r="A71" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="6"/>
+      <c r="T71" s="6"/>
+    </row>
+    <row r="72" spans="1:20">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>358</v>
+      </c>
+      <c r="H72" t="s">
+        <v>359</v>
+      </c>
+      <c r="K72" t="s">
+        <v>39</v>
+      </c>
+      <c r="N72" t="s">
         <v>288</v>
       </c>
-      <c r="R59" t="s">
+      <c r="R72" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="73" spans="1:20" s="5" customFormat="1">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="6"/>
+      <c r="T73" s="6"/>
+    </row>
+    <row r="74" spans="1:20" s="5" customFormat="1">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="6"/>
+      <c r="T74" s="6"/>
+    </row>
+    <row r="75" spans="1:20" s="5" customFormat="1">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+      <c r="P75" s="6"/>
+      <c r="Q75" s="6"/>
+      <c r="R75" s="6"/>
+      <c r="S75" s="6"/>
+      <c r="T75" s="6"/>
+    </row>
+    <row r="76" spans="1:20" s="5" customFormat="1">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="6"/>
+      <c r="T76" s="6"/>
+    </row>
+    <row r="80" spans="1:20">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5951,7 +6384,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -6811,7 +7244,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>